<commit_message>
Corecteaza doua cerinte din lista
</commit_message>
<xml_diff>
--- a/docs/lab01/Lab01_ReviewReport.xlsx
+++ b/docs/lab01/Lab01_ReviewReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\facultate-repo\sem6\vvss\tasks-verification-and-validation\docs\lab01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cosmin Popa\Desktop\cursuri si altele\anul 3\sem 2\Verificarea si validarea sistemelor soft\Laborator\lab\tasks-verification-and-validation\docs\lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB3CEFE-B555-4E48-822F-CB89CA42964B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1938D8B5-0DB7-4ECD-AB2E-01504735D7DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="650" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="64">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -213,19 +213,41 @@
   </si>
   <si>
     <t>No need for else; either the function enters the if and then returns or just returns. Removed else.</t>
+  </si>
+  <si>
+    <t>F01</t>
+  </si>
+  <si>
+    <t>F04</t>
+  </si>
+  <si>
+    <t>Cosmin-Mihai Popa</t>
+  </si>
+  <si>
+    <t>Cerinta trebuie sa ofere clarificari suplimentare cu privire la gestionarea task-urilor repetitive. Mai exact, trebuie specificat modul in care se gestioneaza intervalul de timp pentru task-urile care se repeta la intervale regulate.</t>
+  </si>
+  <si>
+    <t>Cerinta trebuie sa clarifice modul in care sunt modificate detaliile unui task repetitiv. Trebuie specificat daca se modifica toate instantele unui task repetitiv, sau doar instanta specifica.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -404,79 +426,80 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -786,23 +809,23 @@
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="6"/>
-    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.28515625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.85546875" style="6"/>
+    <col min="1" max="1" width="8.81640625" style="6"/>
+    <col min="2" max="2" width="12.26953125" style="6" customWidth="1"/>
+    <col min="3" max="4" width="16.26953125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.453125" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.81640625" style="6"/>
     <col min="9" max="9" width="21" style="6" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" style="6" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="6"/>
+    <col min="10" max="10" width="14.453125" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="8.81640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -813,7 +836,7 @@
       <c r="I1" s="23"/>
       <c r="J1" s="23"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B2" s="24" t="s">
         <v>19</v>
       </c>
@@ -828,14 +851,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I3" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="J3" s="17">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C4" s="13" t="s">
         <v>0</v>
       </c>
@@ -849,7 +876,7 @@
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
@@ -863,7 +890,7 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
@@ -871,14 +898,14 @@
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="22"/>
       <c r="E7" s="22"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -892,24 +919,36 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B25" si="0">B11+1</f>
         <v>3</v>
@@ -918,7 +957,7 @@
       <c r="D12" s="1"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -927,7 +966,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -936,7 +975,7 @@
       <c r="D14" s="1"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -945,7 +984,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -954,7 +993,7 @@
       <c r="D16" s="1"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -963,7 +1002,7 @@
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -972,7 +1011,7 @@
       <c r="D18" s="3"/>
       <c r="E18" s="15"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -981,7 +1020,7 @@
       <c r="D19" s="3"/>
       <c r="E19" s="15"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -990,7 +1029,7 @@
       <c r="D20" s="3"/>
       <c r="E20" s="15"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -999,7 +1038,7 @@
       <c r="D21" s="3"/>
       <c r="E21" s="15"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1008,7 +1047,7 @@
       <c r="D22" s="3"/>
       <c r="E22" s="15"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1017,7 +1056,7 @@
       <c r="D23" s="3"/>
       <c r="E23" s="15"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1026,7 +1065,7 @@
       <c r="D24" s="3"/>
       <c r="E24" s="15"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1035,7 +1074,7 @@
       <c r="D25" s="3"/>
       <c r="E25" s="15"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C27" s="11" t="s">
         <v>8</v>
       </c>
@@ -1067,18 +1106,18 @@
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="6"/>
-    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.28515625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.85546875" style="6"/>
+    <col min="1" max="1" width="8.81640625" style="6"/>
+    <col min="2" max="2" width="12.26953125" style="6" customWidth="1"/>
+    <col min="3" max="4" width="16.26953125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.453125" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.81640625" style="6"/>
     <col min="9" max="9" width="22" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="6"/>
+    <col min="10" max="16384" width="8.81640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -1089,7 +1128,7 @@
       <c r="I1" s="23"/>
       <c r="J1" s="23"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B2" s="24" t="s">
         <v>18</v>
       </c>
@@ -1104,14 +1143,14 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
       <c r="I3" s="17"/>
       <c r="J3" s="17"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
@@ -1125,7 +1164,7 @@
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
@@ -1139,7 +1178,7 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
@@ -1147,14 +1186,14 @@
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="22"/>
       <c r="E7" s="22"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1168,7 +1207,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1176,7 +1215,7 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1185,7 +1224,7 @@
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
@@ -1194,7 +1233,7 @@
       <c r="D12" s="1"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1203,7 +1242,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1212,7 +1251,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1221,7 +1260,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1230,7 +1269,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1239,7 +1278,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1248,7 +1287,7 @@
       <c r="D18" s="1"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1257,7 +1296,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1266,7 +1305,7 @@
       <c r="D20" s="1"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1275,7 +1314,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1284,7 +1323,7 @@
       <c r="D22" s="1"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1293,7 +1332,7 @@
       <c r="D23" s="1"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1302,7 +1341,7 @@
       <c r="D24" s="1"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1311,7 +1350,7 @@
       <c r="D25" s="1"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1320,7 +1359,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C28" s="11" t="s">
         <v>8</v>
       </c>
@@ -1348,23 +1387,23 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="6"/>
-    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.85546875" style="6"/>
-    <col min="9" max="9" width="26.7109375" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="6"/>
+    <col min="1" max="1" width="8.81640625" style="6"/>
+    <col min="2" max="2" width="12.26953125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.26953125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="20.7265625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.453125" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.81640625" style="6"/>
+    <col min="9" max="9" width="26.7265625" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.81640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -1375,7 +1414,7 @@
       <c r="I1" s="23"/>
       <c r="J1" s="23"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B2" s="24" t="s">
         <v>17</v>
       </c>
@@ -1390,7 +1429,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
@@ -1401,7 +1440,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
@@ -1415,7 +1454,7 @@
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
@@ -1429,7 +1468,7 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
@@ -1439,7 +1478,7 @@
       </c>
       <c r="E6" s="22"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
@@ -1448,7 +1487,7 @@
       </c>
       <c r="E7" s="22"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1462,7 +1501,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1476,7 +1515,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1491,7 +1530,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
@@ -1506,7 +1545,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1521,7 +1560,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1536,7 +1575,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1551,7 +1590,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1566,7 +1605,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1581,7 +1620,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1596,7 +1635,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1605,7 +1644,7 @@
       <c r="D19" s="1"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1614,7 +1653,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1623,7 +1662,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1632,7 +1671,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1641,7 +1680,7 @@
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1650,7 +1689,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1659,7 +1698,7 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1668,7 +1707,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1677,7 +1716,7 @@
       <c r="D27" s="2"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1686,7 +1725,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1695,7 +1734,7 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1704,7 +1743,7 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C32" s="11" t="s">
         <v>8</v>
       </c>
@@ -1738,20 +1777,20 @@
       <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="6"/>
-    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="8.81640625" style="6"/>
+    <col min="2" max="2" width="12.26953125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.26953125" style="6" customWidth="1"/>
     <col min="4" max="4" width="18" style="6" customWidth="1"/>
     <col min="5" max="5" width="24" style="6" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" style="6" customWidth="1"/>
-    <col min="7" max="8" width="8.85546875" style="6"/>
-    <col min="9" max="9" width="26.7109375" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="6"/>
+    <col min="6" max="6" width="16.54296875" style="6" customWidth="1"/>
+    <col min="7" max="8" width="8.81640625" style="6"/>
+    <col min="9" max="9" width="26.7265625" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.81640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -1762,7 +1801,7 @@
       <c r="I1" s="23"/>
       <c r="J1" s="23"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B2" s="24" t="s">
         <v>31</v>
       </c>
@@ -1777,14 +1816,14 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
       <c r="I3" s="17"/>
       <c r="J3" s="17"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C4" s="16" t="s">
         <v>25</v>
       </c>
@@ -1796,7 +1835,7 @@
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
@@ -1808,7 +1847,7 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>1</v>
@@ -1817,7 +1856,7 @@
       <c r="E6" s="22"/>
       <c r="F6" s="20"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1834,7 +1873,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1843,7 +1882,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1853,7 +1892,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
@@ -1863,7 +1902,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1873,7 +1912,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1883,7 +1922,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1893,7 +1932,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1903,7 +1942,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1913,7 +1952,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1923,7 +1962,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1933,7 +1972,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1943,7 +1982,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1953,7 +1992,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1963,7 +2002,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1973,7 +2012,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1983,7 +2022,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1993,7 +2032,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2003,7 +2042,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2013,7 +2052,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2023,7 +2062,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2033,7 +2072,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2043,7 +2082,7 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.35">
       <c r="C32" s="34" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
Fixed some issues with SonarLint code analysis tool and added the class diagrams
</commit_message>
<xml_diff>
--- a/docs/lab01/Lab01_ReviewReport.xlsx
+++ b/docs/lab01/Lab01_ReviewReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cosmin Popa\Desktop\cursuri si altele\anul 3\sem 2\Verificarea si validarea sistemelor soft\Laborator\lab\tasks-verification-and-validation\docs\lab01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\tasks-verification-and-validation\docs\lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1938D8B5-0DB7-4ECD-AB2E-01504735D7DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6571C550-D008-4870-A506-5CFE051C1403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="81">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -179,9 +179,6 @@
     <t>The variable name is tks instead of tasks. At first view, anyone who read the code might get confused because tks does not really have a meaning.</t>
   </si>
   <si>
-    <t>1h</t>
-  </si>
-  <si>
     <t>LinkedTaskList.java/15</t>
   </si>
   <si>
@@ -228,19 +225,159 @@
   </si>
   <si>
     <t>Cerinta trebuie sa clarifice modul in care sunt modificate detaliile unui task repetitiv. Trebuie specificat daca se modifica toate instantele unui task repetitiv, sau doar instanta specifica.</t>
+  </si>
+  <si>
+    <t>22.03.2024</t>
+  </si>
+  <si>
+    <t>Petec Răzvan-Gabriel</t>
+  </si>
+  <si>
+    <t>22.03.2023</t>
+  </si>
+  <si>
+    <t>0.5h</t>
+  </si>
+  <si>
+    <t>SonarLint</t>
+  </si>
+  <si>
+    <t>Cognitive Complexity of methods should not be too high</t>
+  </si>
+  <si>
+    <t>Task.java, 112-156</t>
+  </si>
+  <si>
+    <t>public Date nextTimeAfter(Date current)
+    {
+        if (current.after(end) || current.equals(end))
+        {
+            return null;
+        }
+        if (!isActive())
+        {
+            return null;
+        }
+        if (isRepeated())
+        {
+            if (current.before(start))
+            {
+                return start;
+            }
+            Date timeBefore = start;
+            Date timeAfter = start;
+            for (long i = start.getTime(); i &lt;= end.getTime(); i += interval * 1000L)
+            {
+                if (current.equals(timeAfter))
+                {
+                    return new Date(timeAfter.getTime() + interval * 1000L);
+                }
+                if (current.after(timeBefore) &amp;&amp; current.before(timeAfter))
+                {
+                    return timeAfter;
+                }
+                timeBefore = timeAfter;
+                timeAfter = new Date(timeAfter.getTime() + interval * 1000L);
+            }
+        }
+        if (!isRepeated() &amp;&amp; current.before(time))
+        {
+            return time;
+        }
+        return null;
+    }</t>
+  </si>
+  <si>
+    <t>Divided the logic into multiple functions:
+private boolean isDateValid(Date current) {
+        return !(current.equals(end) || current.after(end) || !isActive());
+    }
+    private Date loopDates(Date current) {
+        Date timeBefore = start;
+        Date timeAfter = start;
+        for (long i = start.getTime(); i &lt;= end.getTime(); i += interval * 1000L) {
+            if (current.equals(timeAfter)) {
+                return new Date(timeAfter.getTime() + interval * 1000L);
+            }
+            if (current.after(timeBefore) &amp;&amp; current.before(timeAfter)) {
+                return timeAfter;
+            }
+            timeBefore = timeAfter;
+            timeAfter = new Date(timeAfter.getTime() + interval * 1000L);
+        }
+        return null;
+    }
+    public Date nextTimeAfter(Date current) {
+        if (!isDateValid(current)) {
+            return null;
+        }
+        if (isRepeated()) {
+            if (current.before(start)) {
+                return start;
+            }
+            return loopDates(current);
+        } else if (current.before(time)) {
+            return time;
+        }
+        return null;
+    }</t>
+  </si>
+  <si>
+    <t>DateService.java, 34</t>
+  </si>
+  <si>
+    <t>DateService.java, 41</t>
+  </si>
+  <si>
+    <t>static base class members should not be accessed via derived types</t>
+  </si>
+  <si>
+    <t>Calendar calendar = GregorianCalendar.getInstance();</t>
+  </si>
+  <si>
+    <t>Called the method from the original class, as it's not overriden:
+Calendar calendar = Calendar.getInstance();</t>
+  </si>
+  <si>
+    <t>Main.Java, 21-22</t>
+  </si>
+  <si>
+    <t>Constant names should comply with a naming convention</t>
+  </si>
+  <si>
+    <t>private static final int defaultWidth = 820;
+private static final int defaultHeight = 520;</t>
+  </si>
+  <si>
+    <t>private static final int DEFAULT_WIDTH = 820;
+private static final int DEFAULT_HEIGHT = 520;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -322,6 +459,19 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFCF8E6D"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -426,80 +576,97 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -515,6 +682,143 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>361949</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>85522</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB535E7D-BC9E-DFB6-81F4-1CF737A40013}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="361949" y="6505574"/>
+          <a:ext cx="4800601" cy="6162473"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>47626</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3217043</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>155864</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9408FFA3-74F3-845C-501E-ECA5525CF2C3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5326207" y="11356399"/>
+          <a:ext cx="7692927" cy="3918238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>397565</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>66262</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>163286</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>160104</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FAB688EE-9249-C82E-0CDC-0F9F8892B5BD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5336958" y="16517298"/>
+          <a:ext cx="7861971" cy="4094342"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -809,40 +1113,40 @@
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" style="6"/>
-    <col min="2" max="2" width="12.26953125" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.26953125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.453125" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.81640625" style="6"/>
+    <col min="1" max="1" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
+    <col min="3" max="4" width="16.28515625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.85546875" style="6"/>
     <col min="9" max="9" width="21" style="6" customWidth="1"/>
-    <col min="10" max="10" width="14.453125" style="6" customWidth="1"/>
-    <col min="11" max="16384" width="8.81640625" style="6"/>
+    <col min="10" max="10" width="14.42578125" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B2" s="24" t="s">
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -851,61 +1155,65 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="36" t="s">
-        <v>61</v>
+      <c r="I3" s="22" t="s">
+        <v>60</v>
       </c>
       <c r="J3" s="17">
         <v>235</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="25"/>
+      <c r="E4" s="28"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="27"/>
+      <c r="E5" s="30"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D6" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="25"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D7" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="25"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -919,36 +1227,36 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D10" s="1">
         <v>1</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D11" s="1">
         <v>1</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B25" si="0">B11+1</f>
         <v>3</v>
@@ -957,7 +1265,7 @@
       <c r="D12" s="1"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -966,7 +1274,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -975,7 +1283,7 @@
       <c r="D14" s="1"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -984,7 +1292,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -993,7 +1301,7 @@
       <c r="D16" s="1"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1002,7 +1310,7 @@
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1011,7 +1319,7 @@
       <c r="D18" s="3"/>
       <c r="E18" s="15"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1020,7 +1328,7 @@
       <c r="D19" s="3"/>
       <c r="E19" s="15"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1029,7 +1337,7 @@
       <c r="D20" s="3"/>
       <c r="E20" s="15"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1038,7 +1346,7 @@
       <c r="D21" s="3"/>
       <c r="E21" s="15"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1047,7 +1355,7 @@
       <c r="D22" s="3"/>
       <c r="E22" s="15"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1056,7 +1364,7 @@
       <c r="D23" s="3"/>
       <c r="E23" s="15"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1065,7 +1373,7 @@
       <c r="D24" s="3"/>
       <c r="E24" s="15"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1074,12 +1382,14 @@
       <c r="D25" s="3"/>
       <c r="E25" s="15"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C27" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D27" s="12"/>
-      <c r="E27" s="1"/>
+      <c r="E27" s="1" t="s">
+        <v>66</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1103,38 +1413,38 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" style="6"/>
-    <col min="2" max="2" width="12.26953125" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.26953125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.453125" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.81640625" style="6"/>
+    <col min="1" max="1" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
+    <col min="3" max="4" width="16.28515625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.85546875" style="6"/>
     <col min="9" max="9" width="22" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.81640625" style="6"/>
+    <col min="10" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B2" s="24" t="s">
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1143,57 +1453,65 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I3" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="J3" s="17">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="28"/>
+      <c r="E4" s="31"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="30"/>
+      <c r="E5" s="33"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D6" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6" s="25"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D7" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" s="25"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1207,7 +1525,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1215,7 +1533,7 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1224,7 +1542,7 @@
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
@@ -1233,7 +1551,7 @@
       <c r="D12" s="1"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1242,7 +1560,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1251,7 +1569,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1260,7 +1578,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1269,7 +1587,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1278,7 +1596,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1287,7 +1605,7 @@
       <c r="D18" s="1"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1296,7 +1614,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1305,7 +1623,7 @@
       <c r="D20" s="1"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1314,7 +1632,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1323,7 +1641,7 @@
       <c r="D22" s="1"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1332,7 +1650,7 @@
       <c r="D23" s="1"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1341,7 +1659,7 @@
       <c r="D24" s="1"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1350,7 +1668,7 @@
       <c r="D25" s="1"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1359,7 +1677,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C28" s="11" t="s">
         <v>8</v>
       </c>
@@ -1387,40 +1705,40 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" style="6"/>
-    <col min="2" max="2" width="12.26953125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.26953125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="20.7265625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.453125" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.81640625" style="6"/>
-    <col min="9" max="9" width="26.7265625" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.81640625" style="6"/>
+    <col min="1" max="1" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.85546875" style="6"/>
+    <col min="9" max="9" width="26.7109375" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B2" s="24" t="s">
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1429,7 +1747,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
@@ -1440,54 +1758,54 @@
         <v>235</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="31"/>
+      <c r="E4" s="34"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="33"/>
+      <c r="E5" s="36"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="22"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="E6" s="25"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="22"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="E7" s="25"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1501,7 +1819,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1515,7 +1833,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1530,7 +1848,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
@@ -1545,7 +1863,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1560,7 +1878,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1569,28 +1887,28 @@
         <v>41</v>
       </c>
       <c r="D14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E14" s="2" t="s">
+    </row>
+    <row r="15" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="B15" s="3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="B15" s="3">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1599,13 +1917,13 @@
         <v>37</v>
       </c>
       <c r="D16" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1614,13 +1932,13 @@
         <v>38</v>
       </c>
       <c r="D17" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1629,13 +1947,13 @@
         <v>41</v>
       </c>
       <c r="D18" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1644,7 +1962,7 @@
       <c r="D19" s="1"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1653,7 +1971,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1662,7 +1980,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1671,7 +1989,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1680,7 +1998,7 @@
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1689,7 +2007,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1698,7 +2016,7 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1707,7 +2025,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1716,7 +2034,7 @@
       <c r="D27" s="2"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1725,7 +2043,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1734,7 +2052,7 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1743,13 +2061,13 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C32" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D32" s="12"/>
       <c r="E32" s="1" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1773,41 +2091,41 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" style="6"/>
-    <col min="2" max="2" width="12.26953125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.26953125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="18" style="6" customWidth="1"/>
-    <col min="5" max="5" width="24" style="6" customWidth="1"/>
-    <col min="6" max="6" width="16.54296875" style="6" customWidth="1"/>
-    <col min="7" max="8" width="8.81640625" style="6"/>
-    <col min="9" max="9" width="26.7265625" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.81640625" style="6"/>
+    <col min="1" max="1" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="30.5703125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="72.85546875" style="6" customWidth="1"/>
+    <col min="6" max="6" width="48.5703125" style="6" customWidth="1"/>
+    <col min="7" max="8" width="8.85546875" style="6"/>
+    <col min="9" max="9" width="26.7109375" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B2" s="24" t="s">
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1816,47 +2134,57 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I3" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="J3" s="17">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
+      <c r="D4" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="34"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
+      <c r="D5" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" s="25"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
+      <c r="D6" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E6" s="25"/>
       <c r="F6" s="20"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1873,56 +2201,88 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C10" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C11" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E11" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="F11" s="41" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C12" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E12" s="40" t="s">
+        <v>75</v>
+      </c>
+      <c r="F12" s="41" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C13" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E13" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="F13" s="43" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="E14" s="42"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1932,7 +2292,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1942,7 +2302,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1952,7 +2312,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1962,7 +2322,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1972,7 +2332,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1982,7 +2342,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1992,7 +2352,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -2002,7 +2362,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2012,7 +2372,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2022,7 +2382,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2032,7 +2392,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2042,7 +2402,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2052,7 +2412,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2062,7 +2422,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2072,7 +2432,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2082,12 +2442,12 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C32" s="34" t="s">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C32" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="35"/>
-      <c r="E32" s="35"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="38"/>
       <c r="F32" s="18"/>
     </row>
   </sheetData>
@@ -2101,5 +2461,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed the diagrams and renamed the global controller
</commit_message>
<xml_diff>
--- a/docs/lab01/Lab01_ReviewReport.xlsx
+++ b/docs/lab01/Lab01_ReviewReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\tasks-verification-and-validation\docs\lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6571C550-D008-4870-A506-5CFE051C1403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{773BDF1B-FC3F-43E1-8FA8-EF9F1A05F443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11505" yWindow="3015" windowWidth="21600" windowHeight="11295" tabRatio="650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="89">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -132,9 +132,6 @@
   </si>
   <si>
     <t>Tool-based Code Analysis</t>
-  </si>
-  <si>
-    <t>Effort to perform tool-based code analysis (hours):</t>
   </si>
   <si>
     <t>Panduru Mihai</t>
@@ -351,6 +348,33 @@
   <si>
     <t>private static final int DEFAULT_WIDTH = 820;
 private static final int DEFAULT_HEIGHT = 520;</t>
+  </si>
+  <si>
+    <t>Effort to perform tool-based code analysis (hours): 0.5h</t>
+  </si>
+  <si>
+    <t>A03</t>
+  </si>
+  <si>
+    <t>The TaskList class has a method getAll(), this metod is not mentioned in the class diagram, but the getter is there, either mention them all or none.</t>
+  </si>
+  <si>
+    <t>ClassDiagramTasks_v1.0.png</t>
+  </si>
+  <si>
+    <t>ClassDiagramDepTasks_v1.0.png</t>
+  </si>
+  <si>
+    <t>The Task class has an attribute called "interval", but in this diagram, it does not.</t>
+  </si>
+  <si>
+    <t>A07</t>
+  </si>
+  <si>
+    <t>Both</t>
+  </si>
+  <si>
+    <t>The Controller class is too unclear, considering the fact that there are multiple controllers in the application. Renamed the class to "GlobalController".</t>
   </si>
 </sst>
 </file>
@@ -609,6 +633,19 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -654,19 +691,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -689,15 +713,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>361949</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>19049</xdr:rowOff>
+      <xdr:colOff>328819</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>101875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>85522</xdr:rowOff>
+      <xdr:colOff>185945</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>168348</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -720,8 +744,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="361949" y="6505574"/>
-          <a:ext cx="4800601" cy="6162473"/>
+          <a:off x="328819" y="12931636"/>
+          <a:ext cx="4801843" cy="6162473"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -733,15 +757,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>47626</xdr:rowOff>
+      <xdr:colOff>365677</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>55908</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>3217043</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>155864</xdr:rowOff>
+      <xdr:colOff>3192195</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>164146</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -764,8 +788,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5326207" y="11356399"/>
-          <a:ext cx="7692927" cy="3918238"/>
+          <a:off x="5310394" y="12885669"/>
+          <a:ext cx="7688410" cy="3918238"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -777,15 +801,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>397565</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:colOff>364435</xdr:colOff>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>66262</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>163286</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>160104</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3188805</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>66491</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -808,8 +832,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5336958" y="16517298"/>
-          <a:ext cx="7861971" cy="4094342"/>
+          <a:off x="5309152" y="16896523"/>
+          <a:ext cx="7686262" cy="4000729"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1134,19 +1158,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1160,7 +1184,7 @@
         <v>20</v>
       </c>
       <c r="I3" s="22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J3" s="17">
         <v>235</v>
@@ -1170,10 +1194,10 @@
       <c r="C4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="28"/>
+      <c r="E4" s="33"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
@@ -1184,10 +1208,10 @@
       <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="30"/>
+      <c r="E5" s="35"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -1199,19 +1223,19 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="E6" s="25"/>
+      <c r="D6" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="30"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="E7" s="25"/>
+      <c r="D7" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="30"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
@@ -1232,13 +1256,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D10" s="1">
         <v>1</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -1247,13 +1271,13 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D11" s="1">
         <v>1</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1388,7 +1412,7 @@
       </c>
       <c r="D27" s="12"/>
       <c r="E27" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1412,7 +1436,7 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
@@ -1432,19 +1456,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1458,7 +1482,7 @@
         <v>20</v>
       </c>
       <c r="I3" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J3" s="17">
         <v>235</v>
@@ -1468,10 +1492,10 @@
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="31"/>
+      <c r="E4" s="36"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
@@ -1482,10 +1506,10 @@
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="33"/>
+      <c r="E5" s="38"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -1497,19 +1521,19 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="E6" s="25"/>
+      <c r="D6" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" s="30"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="E7" s="25"/>
+      <c r="D7" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" s="30"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
@@ -1525,31 +1549,49 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
+      <c r="C12" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
@@ -1682,7 +1724,9 @@
         <v>8</v>
       </c>
       <c r="D28" s="12"/>
-      <c r="E28" s="1"/>
+      <c r="E28" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1726,19 +1770,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1752,7 +1796,7 @@
         <v>20</v>
       </c>
       <c r="I3" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J3" s="17">
         <v>235</v>
@@ -1762,10 +1806,10 @@
       <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="34"/>
+      <c r="E4" s="39"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
@@ -1776,10 +1820,10 @@
       <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="36"/>
+      <c r="E5" s="41"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -1791,19 +1835,19 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="25"/>
+      <c r="D6" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="30"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="25"/>
+      <c r="D7" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="30"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
@@ -1824,13 +1868,13 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -1839,13 +1883,13 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1854,13 +1898,13 @@
         <v>3</v>
       </c>
       <c r="C12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -1869,13 +1913,13 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1884,13 +1928,13 @@
         <v>5</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -1899,13 +1943,13 @@
         <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1914,13 +1958,13 @@
         <v>7</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="45" x14ac:dyDescent="0.25">
@@ -1929,13 +1973,13 @@
         <v>8</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D17" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="18" spans="2:5" ht="45" x14ac:dyDescent="0.25">
@@ -1944,13 +1988,13 @@
         <v>9</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D18" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
@@ -2067,7 +2111,7 @@
       </c>
       <c r="D32" s="12"/>
       <c r="E32" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -2091,8 +2135,8 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView topLeftCell="A51" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I69" sqref="I69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2113,19 +2157,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -2139,7 +2183,7 @@
         <v>20</v>
       </c>
       <c r="I3" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J3" s="17">
         <v>235</v>
@@ -2149,10 +2193,10 @@
       <c r="C4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="34" t="s">
-        <v>67</v>
-      </c>
-      <c r="E4" s="34"/>
+      <c r="D4" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="39"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
@@ -2163,10 +2207,10 @@
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="E5" s="25"/>
+      <c r="D5" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="30"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -2178,10 +2222,10 @@
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="E6" s="25"/>
+      <c r="D6" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6" s="30"/>
       <c r="F6" s="20"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -2206,16 +2250,16 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2224,16 +2268,16 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="E11" s="39" t="s">
+      <c r="F11" s="26" t="s">
         <v>75</v>
-      </c>
-      <c r="F11" s="41" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2242,16 +2286,16 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="E12" s="40" t="s">
+      <c r="F12" s="26" t="s">
         <v>75</v>
-      </c>
-      <c r="F12" s="41" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2260,16 +2304,16 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="E13" s="41" t="s">
+      <c r="F13" s="28" t="s">
         <v>79</v>
-      </c>
-      <c r="F13" s="43" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -2279,7 +2323,7 @@
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="42"/>
+      <c r="E14" s="27"/>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -2443,11 +2487,11 @@
       <c r="F30" s="2"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C32" s="37" t="s">
-        <v>32</v>
-      </c>
-      <c r="D32" s="38"/>
-      <c r="E32" s="38"/>
+      <c r="C32" s="42" t="s">
+        <v>80</v>
+      </c>
+      <c r="D32" s="43"/>
+      <c r="E32" s="43"/>
       <c r="F32" s="18"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed some of the architectural observations
</commit_message>
<xml_diff>
--- a/docs/lab01/Lab01_ReviewReport.xlsx
+++ b/docs/lab01/Lab01_ReviewReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\tasks-verification-and-validation\docs\lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{773BDF1B-FC3F-43E1-8FA8-EF9F1A05F443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17EB728B-015F-4015-951D-F1D4C4F9032F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11505" yWindow="3015" windowWidth="21600" windowHeight="11295" tabRatio="650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="92">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -336,20 +336,9 @@
 Calendar calendar = Calendar.getInstance();</t>
   </si>
   <si>
-    <t>Main.Java, 21-22</t>
-  </si>
-  <si>
     <t>Constant names should comply with a naming convention</t>
   </si>
   <si>
-    <t>private static final int defaultWidth = 820;
-private static final int defaultHeight = 520;</t>
-  </si>
-  <si>
-    <t>private static final int DEFAULT_WIDTH = 820;
-private static final int DEFAULT_HEIGHT = 520;</t>
-  </si>
-  <si>
     <t>Effort to perform tool-based code analysis (hours): 0.5h</t>
   </si>
   <si>
@@ -362,12 +351,6 @@
     <t>ClassDiagramTasks_v1.0.png</t>
   </si>
   <si>
-    <t>ClassDiagramDepTasks_v1.0.png</t>
-  </si>
-  <si>
-    <t>The Task class has an attribute called "interval", but in this diagram, it does not.</t>
-  </si>
-  <si>
     <t>A07</t>
   </si>
   <si>
@@ -375,13 +358,37 @@
   </si>
   <si>
     <t>The Controller class is too unclear, considering the fact that there are multiple controllers in the application. Renamed the class to "GlobalController".</t>
+  </si>
+  <si>
+    <t>Main.Java, 21</t>
+  </si>
+  <si>
+    <t>Main.Java, 22</t>
+  </si>
+  <si>
+    <t>private static final int defaultWidth = 820;</t>
+  </si>
+  <si>
+    <t>private static final int defaultHeight = 520;</t>
+  </si>
+  <si>
+    <t>private static final int DEFAULT_WIDTH = 820;</t>
+  </si>
+  <si>
+    <t>private static final int DEFAULT_HEIGHT = 520;</t>
+  </si>
+  <si>
+    <t>A01</t>
+  </si>
+  <si>
+    <t>There overall arhitecture doesn't follow the layered pattern; there is controller, domain and service, but no persistence layer (repository), the data is written to the file directly from the controller layer; the service is used only for the Read operation, but not for Create, Update and Delete</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -493,13 +500,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFCF8E6D"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -600,7 +600,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -639,12 +639,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -690,6 +684,9 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1158,19 +1155,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="H1" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1194,10 +1191,10 @@
       <c r="C4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="33"/>
+      <c r="E4" s="31"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
@@ -1208,10 +1205,10 @@
       <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="35"/>
+      <c r="E5" s="33"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -1223,19 +1220,19 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="30"/>
+      <c r="E6" s="28"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="29" t="s">
+      <c r="D7" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="E7" s="30"/>
+      <c r="E7" s="28"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
@@ -1436,8 +1433,8 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1456,19 +1453,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="H1" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1492,10 +1489,10 @@
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="36" t="s">
+      <c r="D4" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="36"/>
+      <c r="E4" s="34"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
@@ -1506,10 +1503,10 @@
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="37" t="s">
+      <c r="D5" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="38"/>
+      <c r="E5" s="36"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -1521,19 +1518,19 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="E6" s="30"/>
+      <c r="E6" s="28"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="E7" s="30"/>
+      <c r="E7" s="28"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
@@ -1554,28 +1551,28 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -1584,13 +1581,13 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1770,19 +1767,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="H1" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1806,10 +1803,10 @@
       <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="39" t="s">
+      <c r="D4" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="39"/>
+      <c r="E4" s="37"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
@@ -1820,10 +1817,10 @@
       <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="40" t="s">
+      <c r="D5" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="41"/>
+      <c r="E5" s="39"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -1835,19 +1832,19 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="30"/>
+      <c r="E6" s="28"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="30"/>
+      <c r="E7" s="28"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
@@ -2135,8 +2132,8 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I69" sqref="I69"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="116" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2157,19 +2154,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="H1" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -2193,10 +2190,10 @@
       <c r="C4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="39" t="s">
+      <c r="D4" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="E4" s="39"/>
+      <c r="E4" s="37"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
@@ -2207,10 +2204,10 @@
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="E5" s="30"/>
+      <c r="E5" s="28"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -2222,10 +2219,10 @@
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="E6" s="30"/>
+      <c r="E6" s="28"/>
       <c r="F6" s="20"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -2304,27 +2301,35 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="E13" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="F13" s="28" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="F13" s="42" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="2"/>
+      <c r="C14" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E14" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="F14" s="42" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
@@ -2487,11 +2492,11 @@
       <c r="F30" s="2"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C32" s="42" t="s">
-        <v>80</v>
-      </c>
-      <c r="D32" s="43"/>
-      <c r="E32" s="43"/>
+      <c r="C32" s="40" t="s">
+        <v>77</v>
+      </c>
+      <c r="D32" s="41"/>
+      <c r="E32" s="41"/>
       <c r="F32" s="18"/>
     </row>
   </sheetData>

</xml_diff>